<commit_message>
Add predict weather modules
</commit_message>
<xml_diff>
--- a/library/AI_modules/commandVoice/commandset.xlsx
+++ b/library/AI_modules/commandVoice/commandset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC47C57C-C270-4F12-A519-6CE2AE33571B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3997CF-0CCB-43EF-8D39-6A0F72545C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B9FC8548-E4F9-4E4F-BFEA-708F626346F8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="299">
   <si>
     <t>Speech</t>
   </si>
@@ -880,6 +880,48 @@
   </si>
   <si>
     <t>turn light off</t>
+  </si>
+  <si>
+    <t>Tôi muốn buộc gió lại cho hương đừng bay đi</t>
+  </si>
+  <si>
+    <t>Sao nó không chạy</t>
+  </si>
+  <si>
+    <t>Con mèo đang vật lộn với quả len</t>
+  </si>
+  <si>
+    <t>turn air conditioner on</t>
+  </si>
+  <si>
+    <t>cooling the air</t>
+  </si>
+  <si>
+    <t>cool air</t>
+  </si>
+  <si>
+    <t>air conditioner on</t>
+  </si>
+  <si>
+    <t>turn air conditioner off</t>
+  </si>
+  <si>
+    <t>off the air</t>
+  </si>
+  <si>
+    <t>off the conditioner</t>
+  </si>
+  <si>
+    <t>on the conditioner</t>
+  </si>
+  <si>
+    <t>too light</t>
+  </si>
+  <si>
+    <t>enough light for me assistant</t>
+  </si>
+  <si>
+    <t>Tôi thấy sáng như vậy là quá đủ hãy tắt đèn đi</t>
   </si>
 </sst>
 </file>
@@ -1244,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10ADCA31-5C78-45C7-9983-12DFBF0D7EC4}">
-  <dimension ref="A1:B277"/>
+  <dimension ref="A1:B291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:B26"/>
+    <sheetView tabSelected="1" topLeftCell="A287" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A292" sqref="A292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3480,6 +3522,118 @@
         <v>200</v>
       </c>
     </row>
+    <row r="278" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A278" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B278" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A279" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B279" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A280" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B280" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A281" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B281" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A282" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B282" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A283" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B283" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A284" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B284" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A285" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B285" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A286" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B286" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A287" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B287" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A288" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B288" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A289" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B289" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A290" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B290" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A291" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B291" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>